<commit_message>
added code for excel utility
</commit_message>
<xml_diff>
--- a/testData/myData.xlsx
+++ b/testData/myData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mySampleAPIProject\testapiproject\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{668F1567-47C0-4A20-B30A-2FB391C11B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4752310D-4704-4045-83F9-4B80EA8266D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{4198DD8C-0914-4D8D-8AFE-E275729511EF}"/>
+    <workbookView xWindow="1812" yWindow="1812" windowWidth="17280" windowHeight="8964" xr2:uid="{4198DD8C-0914-4D8D-8AFE-E275729511EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Create_Users" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -52,6 +52,27 @@
   </si>
   <si>
     <t>Cricketer</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>23000</t>
   </si>
 </sst>
 </file>
@@ -87,8 +108,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069277D0-A800-4881-8BF2-86C0F2C69256}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -414,7 +436,7 @@
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -424,10 +446,13 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -435,10 +460,13 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -446,16 +474,22 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated post script with test Data excel file
</commit_message>
<xml_diff>
--- a/testData/myData.xlsx
+++ b/testData/myData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mySampleAPIProject\testapiproject\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4752310D-4704-4045-83F9-4B80EA8266D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{404042BC-242E-4C51-A5C8-AD6D625AA1FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1812" yWindow="1812" windowWidth="17280" windowHeight="8964" xr2:uid="{4198DD8C-0914-4D8D-8AFE-E275729511EF}"/>
   </bookViews>
@@ -54,9 +54,6 @@
     <t>Cricketer</t>
   </si>
   <si>
-    <t>Salary</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -66,19 +63,25 @@
     <t>3</t>
   </si>
   <si>
-    <t>5000</t>
-  </si>
-  <si>
-    <t>10000</t>
-  </si>
-  <si>
-    <t>23000</t>
+    <t>UserID</t>
+  </si>
+  <si>
+    <t>3001</t>
+  </si>
+  <si>
+    <t>3002</t>
+  </si>
+  <si>
+    <t>3003</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -108,9 +111,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,7 +432,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -447,12 +451,12 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -460,13 +464,13 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -474,13 +478,13 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -488,11 +492,12 @@
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>